<commit_message>
ignore images not in timing df and incorrect files in the folder
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orenyang/Documents/UCSD_Lab/xuv_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orenyang/Documents/GitHub/xuv_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7E3A03-52AC-DC4A-BF77-9250101E871C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27E7103-31FD-2A4B-94E5-4E90B4C83D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="820" windowWidth="23740" windowHeight="17360" xr2:uid="{4927715F-6AFE-DE4D-A63B-23B4F008C1CE}"/>
+    <workbookView xWindow="5400" yWindow="780" windowWidth="23740" windowHeight="17360" xr2:uid="{4927715F-6AFE-DE4D-A63B-23B4F008C1CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BE41F7-4675-8243-966B-24771B528980}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,7 +451,7 @@
     <col min="1" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -464,19 +464,13 @@
       <c r="D1">
         <v>2530</v>
       </c>
-      <c r="E1">
-        <v>2531</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -484,7 +478,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -492,7 +486,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -500,22 +494,22 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
made it so good, added gui
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orenyang/Documents/GitHub/xuv_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orenyang/Documents/GitHub/xuv-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27E7103-31FD-2A4B-94E5-4E90B4C83D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5A4C39-46D2-2A49-8F31-00F86F3C63A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="780" windowWidth="23740" windowHeight="17360" xr2:uid="{4927715F-6AFE-DE4D-A63B-23B4F008C1CE}"/>
+    <workbookView xWindow="-1020" yWindow="1240" windowWidth="10000" windowHeight="16700" xr2:uid="{4927715F-6AFE-DE4D-A63B-23B4F008C1CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,33 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>mcp1 frame 1</t>
+    <t>shot</t>
   </si>
   <si>
-    <t>mcp1 frame 2</t>
+    <t>sch frame 1</t>
   </si>
   <si>
-    <t>mcp1 frame 3</t>
-  </si>
-  <si>
-    <t>mcp1 frame 4</t>
-  </si>
-  <si>
-    <t>mcp2 frame 1</t>
-  </si>
-  <si>
-    <t>mcp2 frame 2</t>
-  </si>
-  <si>
-    <t>mcp2 frame 3</t>
-  </si>
-  <si>
-    <t>mcp2 frame 4</t>
-  </si>
-  <si>
-    <t>shot</t>
+    <t>sch frame 2</t>
   </si>
 </sst>
 </file>
@@ -440,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BE41F7-4675-8243-966B-24771B528980}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,67 +433,52 @@
     <col min="1" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1">
-        <v>2528</v>
+        <v>2661</v>
       </c>
       <c r="C1">
-        <v>2529</v>
+        <v>2659</v>
       </c>
       <c r="D1">
-        <v>2530</v>
+        <v>2615</v>
+      </c>
+      <c r="E1">
+        <v>2614</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="C2">
+        <v>51.9</v>
+      </c>
+      <c r="D2">
+        <v>47.5</v>
+      </c>
+      <c r="E2">
+        <v>85.7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
+        <v>97.6</v>
+      </c>
+      <c r="C3">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="D3">
+        <v>77.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>